<commit_message>
csv con 70 preguntas
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="320">
   <si>
     <t>selectionUniq</t>
   </si>
@@ -197,6 +197,789 @@
   </si>
   <si>
     <t>Los sistemas finales utilizan números de puerto para seleccionar la aplicación adecuada. ¿Cuál es el número de puerto mínimo que el sistema host puede asignar dinámicamente?</t>
+  </si>
+  <si>
+    <t>Ha asignado el bloque de direcciones 10.255.255.224 /28 para crear las direcciones de red destinadas a los enlaces WAN punto a punto. ¿Cuántas de estas WANs puede soportar con este bloque de direcciones?</t>
+  </si>
+  <si>
+    <t>Un host en la sucursal sur no puede acceder al servidor con la dirección 192.168.254.222/224. Examinando el host, determina que su dirección IPv4 es 169.254.11.15/16. ¿Cuál es aparentemente el problema?</t>
+  </si>
+  <si>
+    <t>El host está utilizando una dirección de enlace local.</t>
+  </si>
+  <si>
+    <t>El servidor está utilizando una máscara de subred errónea.</t>
+  </si>
+  <si>
+    <t>Se ha asignado una dirección de broadcast al host.</t>
+  </si>
+  <si>
+    <t>El servidor piensa que el host está en la red lógica con el servidor.</t>
+  </si>
+  <si>
+    <t>Indique dos razones para planificar y documentar las direcciones IPv4.</t>
+  </si>
+  <si>
+    <t>B,C</t>
+  </si>
+  <si>
+    <t>Evitar la duplicación de direcciones.</t>
+  </si>
+  <si>
+    <t>Monitorizar la seguridad y el rendimiento.</t>
+  </si>
+  <si>
+    <t>Elegir las direcciones que se quieren</t>
+  </si>
+  <si>
+    <t>Usar las direcciones 200 que son mas rapidas</t>
+  </si>
+  <si>
+    <t>¿Cuál fue la principal motivación para el desarrollo de IPv6?</t>
+  </si>
+  <si>
+    <t>El principal motivo del desarrollo de IPv6 es el agotamiento de las direcciones IPv4.</t>
+  </si>
+  <si>
+    <t>El principal motivo es tener dos Ips más</t>
+  </si>
+  <si>
+    <t>El principal motivo es extender la IPv5.</t>
+  </si>
+  <si>
+    <t>El principal motivo es garantizar que todas las Ips termiunen en 6</t>
+  </si>
+  <si>
+    <t>Enumere factores que han de tenerse en cuenta a la hora de planificar un esquema de direccionamiento IPv4.</t>
+  </si>
+  <si>
+    <t>Agrupe basándose en una ubicación geográfica común.</t>
+  </si>
+  <si>
+    <t>Agrupe los hosts que se utilizan para propósitos comunes.</t>
+  </si>
+  <si>
+    <t>Agrupe basándose en la propiedad.</t>
+  </si>
+  <si>
+    <t>Agrupe basándose en los números.</t>
+  </si>
+  <si>
+    <t>A,B,D</t>
+  </si>
+  <si>
+    <t>¿Cuáles son las tres pruebas que hacen uso de la utilidad ping para comprobar y verificar el funcionamiento de un host?</t>
+  </si>
+  <si>
+    <t>Ping a un host de una red local: prueba el gateway predeterminado del dispositivo.</t>
+  </si>
+  <si>
+    <t>Ping a la dirección de gateway de host u otro host en la misma red: para determinar la comunicación sobre la red local.</t>
+  </si>
+  <si>
+    <t>A,C,D</t>
+  </si>
+  <si>
+    <t>Ping a un host de una red remota: prueba el gateway predeterminado del dispositivo y más allá.</t>
+  </si>
+  <si>
+    <t>Ping 127.0.0.1: prueba de loopback para probar el funcionamiento IP.</t>
+  </si>
+  <si>
+    <t>¿Cuáles son los tipos de mensajes ICMP?</t>
+  </si>
+  <si>
+    <t>Confirmación de host.</t>
+  </si>
+  <si>
+    <t>Destino o servicio inalcanzable.</t>
+  </si>
+  <si>
+    <t>Tiempo excedido.</t>
+  </si>
+  <si>
+    <t>Redirección de ruta y Origen saturado.</t>
+  </si>
+  <si>
+    <t>A,B,C,D</t>
+  </si>
+  <si>
+    <t>Si un nodo recibe una trama y la CRC calculada no coincide con el valor que viaja en la FCS, ¿qué acción tomará el nodo?</t>
+  </si>
+  <si>
+    <t>Descartar la trama.</t>
+  </si>
+  <si>
+    <t>Reconstruir la trama a partir del valor de CRC.</t>
+  </si>
+  <si>
+    <t>Reenviar la trama tal como está al siguiente host.</t>
+  </si>
+  <si>
+    <t>Desactiva la interfaz a la que llega la trama.</t>
+  </si>
+  <si>
+    <t>¿Cuáles de los siguientes protocolos son empleados habitualmente por las WANs? (Seleccione dos opciones.)</t>
+  </si>
+  <si>
+    <t>802.11.</t>
+  </si>
+  <si>
+    <t>Ethernet.</t>
+  </si>
+  <si>
+    <t>HDLC.</t>
+  </si>
+  <si>
+    <t>PPP.</t>
+  </si>
+  <si>
+    <t>C,D</t>
+  </si>
+  <si>
+    <t>¿Cuáles son los contenidos del campo de datos en una trama?</t>
+  </si>
+  <si>
+    <t>64 bytes.</t>
+  </si>
+  <si>
+    <t>La PDU de la capa de red.</t>
+  </si>
+  <si>
+    <t>La dirección de origen de capa 2.</t>
+  </si>
+  <si>
+    <t>Los datos procedentes directamente de la aplicación que los generó.</t>
+  </si>
+  <si>
+    <t>¿Cuál es una característica de una MAC basada en el enfrentamiento?</t>
+  </si>
+  <si>
+    <t>Se usa en un medio no compartido.</t>
+  </si>
+  <si>
+    <t>Los nodos compiten por el uso del medio.</t>
+  </si>
+  <si>
+    <t>Deja la MAC a la capa superior.</t>
+  </si>
+  <si>
+    <t>Cada nodo tiene un tiempo específico para usar el medio.</t>
+  </si>
+  <si>
+    <t>¿Cuáles de las siguientes son subcapas de enlace de datos habituales en las LANs? (Seleccione dos opciones.)</t>
+  </si>
+  <si>
+    <t>Protocolo de unidad de datos.</t>
+  </si>
+  <si>
+    <t>Control de enlace lógico.</t>
+  </si>
+  <si>
+    <t>MAC.</t>
+  </si>
+  <si>
+    <t>Tarjeta de interfaz de red.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes características describe un circuito virtual?</t>
+  </si>
+  <si>
+    <t>Es una técnica para la detección de errores.</t>
+  </si>
+  <si>
+    <t>Proporciona una técnica de encapsulación.</t>
+  </si>
+  <si>
+    <t>Sólo se emplea con topologías físicas punto a punto.</t>
+  </si>
+  <si>
+    <t>Establece una conexión lógica entre dos dispositivos de la red.</t>
+  </si>
+  <si>
+    <t>¿Cuáles de las siguientes funciones lleva a cabo la capa de enlace de datos?</t>
+  </si>
+  <si>
+    <t>Proporciona interfaces de usuario.</t>
+  </si>
+  <si>
+    <t>Garantiza la entrega de datos de extremo a extremo entre los hosts.</t>
+  </si>
+  <si>
+    <t>Conecta el software y el hardware de red.</t>
+  </si>
+  <si>
+    <t>Establece y mantiene sesiones entre las aplicaciones.</t>
+  </si>
+  <si>
+    <t>¿Cuáles de las siguientes afirmaciones acerca de la topología lógica de una red son ciertas?</t>
+  </si>
+  <si>
+    <t>Es siempre multiacceso.</t>
+  </si>
+  <si>
+    <t>Proporciona el direccionamiento físico.</t>
+  </si>
+  <si>
+    <t>Está determinada por la forma en la que están conectados los nodos de la red.</t>
+  </si>
+  <si>
+    <t>Influye en el tipo de MAC usado en la red.</t>
+  </si>
+  <si>
+    <t>Enumere dos protocolos de capa 2.</t>
+  </si>
+  <si>
+    <t>SMTP.</t>
+  </si>
+  <si>
+    <t>HTTP.</t>
+  </si>
+  <si>
+    <t>ATM.</t>
+  </si>
+  <si>
+    <t>A,D</t>
+  </si>
+  <si>
+    <t>¿Cuál es el objetivo de la codificación?</t>
+  </si>
+  <si>
+    <t>Identificar los bits de inicio y de parada en la trama.</t>
+  </si>
+  <si>
+    <t>Designar los conectores de la capa física de las computadoras en relación con la forma en que se conectan al medio de red.</t>
+  </si>
+  <si>
+    <t>Controlar la forma en que las tramas son colocadas en el medio en la capa de enlace de datos.</t>
+  </si>
+  <si>
+    <t>Representar los bits de datos usando diferentes voltajes, patrones de luz u ondas electromagnéticas a medida que son puestos en el medio físico.</t>
+  </si>
+  <si>
+    <t>¿A través de qué proceso el cable UTP ayuda a evitar la diafonía?</t>
+  </si>
+  <si>
+    <t>Apantallando el cable.</t>
+  </si>
+  <si>
+    <t>Trenzando de pares.</t>
+  </si>
+  <si>
+    <t>Conectando a tierra los extremos finales.</t>
+  </si>
+  <si>
+    <t>Revistiendo el cable.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el tipo de conector UTP más común?</t>
+  </si>
+  <si>
+    <t>RJ45</t>
+  </si>
+  <si>
+    <t>JR35</t>
+  </si>
+  <si>
+    <t>UP25</t>
+  </si>
+  <si>
+    <t>J55</t>
+  </si>
+  <si>
+    <t>¿Cuáles de estas opciones describen mejor los objetivos de la capa física?</t>
+  </si>
+  <si>
+    <t>Asegurar una transmisión de datos fiable a través de un enlace físico.</t>
+  </si>
+  <si>
+    <t>Determinar la conectividad y la selección de ruta entre dos sistemas finales.</t>
+  </si>
+  <si>
+    <t>Establecer el direccionamiento físico, la topología de la red y el acceso al medio.</t>
+  </si>
+  <si>
+    <t>Definir las especificaciones funcionales de los enlaces entre los sistemas finales y las señales eléctricas, ópticas y de radio.</t>
+  </si>
+  <si>
+    <t>El cobre es más caro.</t>
+  </si>
+  <si>
+    <t>¿Cuáles son las ventajas de usar cable de fibra óptica en lugar de otro de cobre?</t>
+  </si>
+  <si>
+    <t>Inmunidad a la interferencia electromagnética.</t>
+  </si>
+  <si>
+    <t>Longitud máxima del cable.</t>
+  </si>
+  <si>
+    <t>Mayor ancho de banda potencial.</t>
+  </si>
+  <si>
+    <t>B,C,D</t>
+  </si>
+  <si>
+    <t>¿Cuál es el objetivo del revestimiento en los cables de fibra óptica?</t>
+  </si>
+  <si>
+    <t>Conectar con tierra el cable.</t>
+  </si>
+  <si>
+    <t>Cancelar el ruido.</t>
+  </si>
+  <si>
+    <t>Evitar las pérdidas de luz.</t>
+  </si>
+  <si>
+    <t>Proteger de la EMI.</t>
+  </si>
+  <si>
+    <t>¿Cuáles de las siguientes aseveraciones son ciertas en los cables rectos? (Seleccione dos opciones.)</t>
+  </si>
+  <si>
+    <t>Funcionan en puertos de consola Cisco.</t>
+  </si>
+  <si>
+    <t>Pueden ser 568A ó 568B.</t>
+  </si>
+  <si>
+    <t>Pueden conectar un host con un switch.</t>
+  </si>
+  <si>
+    <t>Pueden conectar dos switches.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes unidades mide la tasa de transferencia de datos real sobre un medio?</t>
+  </si>
+  <si>
+    <t>Salida.</t>
+  </si>
+  <si>
+    <t>Rendimiento.</t>
+  </si>
+  <si>
+    <t>Capacidad de transferencia útil.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes opciones NO es cierta?</t>
+  </si>
+  <si>
+    <t>1 Gbps = 1.000.000.000 bits por segundo.</t>
+  </si>
+  <si>
+    <t>1 kbps = 1000 bits por segundo.</t>
+  </si>
+  <si>
+    <t>1 Mbps = 100.000 bits por segundo.</t>
+  </si>
+  <si>
+    <t>1 Tbps = 1.000.000.000.000 bits por segundo.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes afirmaciones es cierta acerca del (tiempo de bit)?</t>
+  </si>
+  <si>
+    <t>Es el tiempo que se tarda en encapsular los datos de la aplicación en un segmento de bit.</t>
+  </si>
+  <si>
+    <t>Es el tiempo que tarda una NIC en mover un bit desde la capa de enlace de datos al medio de capa 1.</t>
+  </si>
+  <si>
+    <t>Son los estándares IEEE que tienen que ser los mismos en todas las NICs.</t>
+  </si>
+  <si>
+    <t>Es el tiempo que tarda un byte en atravesar el cable de cobre o de fibra.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes direcciones se utiliza como dirección de destino para una trama de broadcast Ethernet?</t>
+  </si>
+  <si>
+    <t>0.0.0.0</t>
+  </si>
+  <si>
+    <t>FF-FF-FF-FF-FF-FF</t>
+  </si>
+  <si>
+    <t>0C-FA-94-24-EF-00</t>
+  </si>
+  <si>
+    <t>¿Cuántos bits tiene una dirección MAC Ethernet?</t>
+  </si>
+  <si>
+    <t>¿Qué campo de una trama Ethernet se utiliza para la detección de errores?</t>
+  </si>
+  <si>
+    <t>Tipo.</t>
+  </si>
+  <si>
+    <t>Preámbulo.</t>
+  </si>
+  <si>
+    <t>FCS.</t>
+  </si>
+  <si>
+    <t>Dirección MAC de destino.</t>
+  </si>
+  <si>
+    <t>¿Qué características Ethernet son compartidas por las versiones históricas de Ethernet y por las heredadas?</t>
+  </si>
+  <si>
+    <t>Mismo tipo de cable.</t>
+  </si>
+  <si>
+    <t>Mismas longitudes de segmento.</t>
+  </si>
+  <si>
+    <t>Misma topología lógica.</t>
+  </si>
+  <si>
+    <t>Mismo coste de instalación.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes opciones describe una conexión a un puerto de un switch?</t>
+  </si>
+  <si>
+    <t>Aísla los broadcasts.</t>
+  </si>
+  <si>
+    <t>Es un dominio de colisión separado.</t>
+  </si>
+  <si>
+    <t>Usa la dirección MAC del puerto del switch como destino.</t>
+  </si>
+  <si>
+    <t>Regenera cada bit que llega a cada puerto del switch.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el estado de operación de un switch Ethernet que crea las entradas de la tabla MAC?</t>
+  </si>
+  <si>
+    <t>Envejecimiento.</t>
+  </si>
+  <si>
+    <t>Filtrado.</t>
+  </si>
+  <si>
+    <t>Inundación.</t>
+  </si>
+  <si>
+    <t>Aprendizaje.</t>
+  </si>
+  <si>
+    <t>Si una trama que llega a un switch contiene una dirección MAC de origen que no está en la tabla MAC, ¿qué proceso tiene lugar?</t>
+  </si>
+  <si>
+    <t>Si una trama que llega a un switch contiene una dirección MAC de destino que no está en la tabla MAC, ¿qué proceso tiene lugar?</t>
+  </si>
+  <si>
+    <t>¿Por qué son más susceptibles al ruido las implementaciones de Ethernet a alta velocidad?</t>
+  </si>
+  <si>
+    <t>Más colisiones.</t>
+  </si>
+  <si>
+    <t>Tiempos de bit más cortos.</t>
+  </si>
+  <si>
+    <t>Operativa full-duplex.</t>
+  </si>
+  <si>
+    <t>Se necesitan cables UTP en lugar de fibra.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes opciones describe una limitación de las tecnologías de Ethernet heredadas?</t>
+  </si>
+  <si>
+    <t>Pobre escalabilidad.</t>
+  </si>
+  <si>
+    <t>Medio caro.</t>
+  </si>
+  <si>
+    <t>Sin colisiones.</t>
+  </si>
+  <si>
+    <t>Formato de trama incompatible con las versiones actuales de Ethernet.</t>
+  </si>
+  <si>
+    <t>Dada la red 178.5.0.0/16 se le ha asignado la tarea de crear tantas subredes como sea posible con al menos 100 hosts. ¿Qué máscara de red utilizaría?</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>255.255.254.0</t>
+  </si>
+  <si>
+    <t>¿Cuál sería la máscara de subred más eficaz si necesitara tantas subredes como fuera posible con 32 hosts cada una?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el rango de host válido para la subred 154.65.128.0 255.255.248.0?</t>
+  </si>
+  <si>
+    <t>154.65.128.1 154.65.128.255</t>
+  </si>
+  <si>
+    <t>154.65.128.1 154.65.135.254</t>
+  </si>
+  <si>
+    <t>154.65.120.1 154.65.135.255</t>
+  </si>
+  <si>
+    <t>154.65.0.0 154.65.255.254</t>
+  </si>
+  <si>
+    <t>100BASE-FX utiliza cableado de fibra y soporta full-duplex hasta una distancia de ________ metros.</t>
+  </si>
+  <si>
+    <t>A,C</t>
+  </si>
+  <si>
+    <t>Servidores.</t>
+  </si>
+  <si>
+    <t>Sistema de audio.</t>
+  </si>
+  <si>
+    <t>Microfono.</t>
+  </si>
+  <si>
+    <t>Administrar el tráfico de broadcast.</t>
+  </si>
+  <si>
+    <t>Requisitos de red parecidos.</t>
+  </si>
+  <si>
+    <t>Especifique dos razones por las que hay que dividir en subredes una red.</t>
+  </si>
+  <si>
+    <t>Un contratista está instalando cable para la red de un nuevo hospital. Las especificaciones del cable exigen que la red esté protegida de la EMI y que tenga un ancho de banda soportado de 1000 Mbps. ¿Qué tipo de cable puede satisfacer estas dos especificaciones?</t>
+  </si>
+  <si>
+    <t>Cable coaxial Thinnet.</t>
+  </si>
+  <si>
+    <t>Cable de fibra óptica.</t>
+  </si>
+  <si>
+    <t>Cable UTP de Categoría 5.</t>
+  </si>
+  <si>
+    <t>Cable coaxial Thicknet.</t>
+  </si>
+  <si>
+    <t>¿Qué dos elementos son necesarios para una configuración inicial de los routers Cisco?</t>
+  </si>
+  <si>
+    <t>Cable cruzado.</t>
+  </si>
+  <si>
+    <t>Cable de consola.</t>
+  </si>
+  <si>
+    <t>Adaptador RJ-15 a DB-9.</t>
+  </si>
+  <si>
+    <t>Software de emulación de terminal.</t>
+  </si>
+  <si>
+    <t>¿Qué comando activa una interfaz de router?</t>
+  </si>
+  <si>
+    <t>Router(config-if)#enable</t>
+  </si>
+  <si>
+    <t>Router(config-if)#no shutdow</t>
+  </si>
+  <si>
+    <t>Router(config-if)#no down</t>
+  </si>
+  <si>
+    <t>Router(config-if)#interface up</t>
+  </si>
+  <si>
+    <t>¿Cuál es el objetivo del comando IOS enable secret?</t>
+  </si>
+  <si>
+    <t>Establecer la protección de la contraseña en las sesiones Telnet entrantes.</t>
+  </si>
+  <si>
+    <t>Establecer la protección de la contraseña en la consola de terminal.</t>
+  </si>
+  <si>
+    <t>Permitir a un usuario el acceso al modo de usuario.</t>
+  </si>
+  <si>
+    <t>Permitir a un usuario introducir una contraseña que será encriptada.</t>
+  </si>
+  <si>
+    <t>¿Qué comando visualizará las estadísticas de todas las interfaces configuradas en un router?</t>
+  </si>
+  <si>
+    <t>list interfaces</t>
+  </si>
+  <si>
+    <t>show interfaces</t>
+  </si>
+  <si>
+    <t>show processes</t>
+  </si>
+  <si>
+    <t>show statistics</t>
+  </si>
+  <si>
+    <t>¿Qué comando mostrará una lista de los comandos disponibles para ver el estado del router?</t>
+  </si>
+  <si>
+    <t>Router#?show</t>
+  </si>
+  <si>
+    <t>Router# sh?</t>
+  </si>
+  <si>
+    <t>Router# show ?</t>
+  </si>
+  <si>
+    <t>Router# status ?</t>
+  </si>
+  <si>
+    <t>¿Para qué puede usarse el puerto de consola? (Seleccione tres opciones.)</t>
+  </si>
+  <si>
+    <t>Depuración.</t>
+  </si>
+  <si>
+    <t>Recuperación de la contraseña</t>
+  </si>
+  <si>
+    <t>Enrutamiento de datos entre las redes.</t>
+  </si>
+  <si>
+    <t>Resolución de problemas.</t>
+  </si>
+  <si>
+    <t>¿Qué usan los routers para seleccionar las mejores rutas para el envío de paquetes?</t>
+  </si>
+  <si>
+    <t>Tablas ARP.</t>
+  </si>
+  <si>
+    <t>Tablas de puenteo.</t>
+  </si>
+  <si>
+    <t>Tablas de enrutamiento.</t>
+  </si>
+  <si>
+    <t>Tablas de conmutación.</t>
+  </si>
+  <si>
+    <t>Seleccione la frase que describe correctamente la memoria flash de un router.</t>
+  </si>
+  <si>
+    <t>Almacena la configuración de inicio predeterminada.</t>
+  </si>
+  <si>
+    <t>Almacena las imágenes del software Cisco IOS.</t>
+  </si>
+  <si>
+    <t>Almacena la información de la tabla de enrutamiento predeterminada.</t>
+  </si>
+  <si>
+    <t>Mantiene la única copia de una imagen del IOS una vez que el router ha arrancado.</t>
+  </si>
+  <si>
+    <t>La capa de aplicación es la ___________ del modelo OSI.</t>
+  </si>
+  <si>
+    <t>Capa 2.</t>
+  </si>
+  <si>
+    <t>Capa 7.</t>
+  </si>
+  <si>
+    <t>Capa 4.</t>
+  </si>
+  <si>
+    <t>Capa 1.</t>
+  </si>
+  <si>
+    <t>¿De qué tres capas OSI consta aproximadamente la capa de aplicación TCP/IP?</t>
+  </si>
+  <si>
+    <t>Aplicación, sesión, transporte.</t>
+  </si>
+  <si>
+    <t>Aplicación, presentación, sesión.</t>
+  </si>
+  <si>
+    <t>Aplicación, transporte, red.</t>
+  </si>
+  <si>
+    <t>Aplicación, red, enlace de datos.</t>
+  </si>
+  <si>
+    <t>¿Qué puerto utiliza el Protocolo de oficina de correos (POP)?</t>
+  </si>
+  <si>
+    <t>Puerto TCP/UDP 53.</t>
+  </si>
+  <si>
+    <t>Puerto TCP 80.</t>
+  </si>
+  <si>
+    <t>Puerto TCP 25.</t>
+  </si>
+  <si>
+    <t>Puerto UDP 110.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el servicio de red más popular?</t>
+  </si>
+  <si>
+    <t>FTP.</t>
+  </si>
+  <si>
+    <t>Telnet.</t>
+  </si>
+  <si>
+    <t>E-mail.</t>
+  </si>
+  <si>
+    <t>FTP requiere ___________ conexión(es) entre el cliente y el servidor para que la transferencia de archivos sea satisfactoria.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>¿Cuál de las siguientes es una conexión utilizando Telnet?</t>
+  </si>
+  <si>
+    <t>Sesión FTP (Protocolo de transferencia de archivos).</t>
+  </si>
+  <si>
+    <t>Sesión TFTP (Protocolo trivial de transferencia de archivos).</t>
+  </si>
+  <si>
+    <t>Sesión VTY (Terminal virtual).</t>
+  </si>
+  <si>
+    <t>Sesión Auxiliar (AUX).</t>
+  </si>
+  <si>
+    <t>Impresoras, teléfonos IP y cámaras IP.</t>
+  </si>
+  <si>
+    <t>Ponga algunos ejemplos de los diferentes tipos de hosts y dispositivos de red que necesitan direcciones IP.</t>
   </si>
 </sst>
 </file>
@@ -300,7 +1083,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -345,6 +1128,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -545,8 +1331,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:H14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Salida">
-  <autoFilter ref="A1:H14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:H71" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Salida">
+  <autoFilter ref="A1:H71"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Type" dataDxfId="7"/>
     <tableColumn id="2" name="ReferenceLayer" dataDxfId="6"/>
@@ -826,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,575 +1992,1487 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
-      <c r="D18"/>
-      <c r="E18"/>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
-      <c r="F19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20"/>
-      <c r="D20"/>
-      <c r="E20"/>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
-    </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
-      <c r="F23"/>
-      <c r="G23"/>
-      <c r="H23"/>
-    </row>
-    <row r="24" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-      <c r="F24"/>
-      <c r="G24"/>
-      <c r="H24"/>
-    </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25"/>
-    </row>
-    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="H26"/>
-    </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27"/>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
-      <c r="H27"/>
-    </row>
-    <row r="28" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
-      <c r="H28"/>
-    </row>
-    <row r="29" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
+    <row r="15" spans="1:8" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="13">
+        <v>2</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="15">
+        <v>4</v>
+      </c>
+      <c r="F15" s="15">
+        <v>7</v>
+      </c>
+      <c r="G15" s="15">
+        <v>14</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="13">
+        <v>2</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="13">
+        <v>2</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="13">
+        <v>2</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="13">
+        <v>2</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="13">
+        <v>2</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="13">
+        <v>2</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="13">
+        <v>3</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="13">
+        <v>3</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="13">
+        <v>3</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="13">
+        <v>3</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="13">
+        <v>3</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="13">
+        <v>3</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="13">
+        <v>3</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="13">
+        <v>3</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="30" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30"/>
-      <c r="G30"/>
-      <c r="H30"/>
-    </row>
-    <row r="31" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-    </row>
-    <row r="32" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32"/>
-      <c r="D32"/>
-      <c r="E32"/>
-      <c r="F32"/>
-      <c r="G32"/>
-      <c r="H32"/>
+      <c r="A30" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" s="13">
+        <v>3</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="13">
+        <v>4</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="13">
+        <v>4</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-    </row>
-    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34"/>
-      <c r="D34"/>
-      <c r="E34"/>
-      <c r="F34"/>
-      <c r="G34"/>
-      <c r="H34"/>
-    </row>
-    <row r="35" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35"/>
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-    </row>
-    <row r="36" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-    </row>
-    <row r="37" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-      <c r="G37"/>
-      <c r="H37"/>
-    </row>
-    <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38"/>
-      <c r="B38"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-    </row>
-    <row r="39" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39"/>
-      <c r="C39"/>
-      <c r="D39"/>
-      <c r="E39"/>
-      <c r="F39"/>
-      <c r="G39"/>
-      <c r="H39"/>
-    </row>
-    <row r="40" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40"/>
-      <c r="C40"/>
-      <c r="D40"/>
-      <c r="E40"/>
-      <c r="F40"/>
-      <c r="G40"/>
-      <c r="H40"/>
-    </row>
-    <row r="41" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41"/>
-      <c r="C41"/>
-      <c r="D41"/>
-      <c r="E41"/>
-      <c r="F41"/>
-      <c r="G41"/>
-      <c r="H41"/>
+      <c r="A33" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="13">
+        <v>4</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="13">
+        <v>4</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="13">
+        <v>4</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="13">
+        <v>4</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="13">
+        <v>4</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="13">
+        <v>4</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="13">
+        <v>4</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="13">
+        <v>4</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="13">
+        <v>4</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" s="16">
+        <v>255255255255</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="42" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42"/>
-      <c r="C42"/>
-      <c r="D42"/>
-      <c r="E42"/>
-      <c r="F42"/>
-      <c r="G42"/>
-      <c r="H42"/>
-    </row>
-    <row r="43" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-    </row>
-    <row r="44" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-    </row>
-    <row r="45" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45"/>
-      <c r="F45"/>
-      <c r="G45"/>
-      <c r="H45"/>
-    </row>
-    <row r="46" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
-    </row>
-    <row r="47" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-    </row>
-    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-    </row>
-    <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="H49"/>
-    </row>
-    <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-    </row>
-    <row r="51" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51"/>
-      <c r="C51"/>
-      <c r="D51"/>
-      <c r="E51"/>
-      <c r="F51"/>
-      <c r="G51"/>
-      <c r="H51"/>
-    </row>
-    <row r="52" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52"/>
-      <c r="B52"/>
-      <c r="C52"/>
-      <c r="D52"/>
-      <c r="E52"/>
-      <c r="F52"/>
-      <c r="G52"/>
-      <c r="H52"/>
-    </row>
-    <row r="53" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53"/>
-      <c r="B53"/>
-      <c r="C53"/>
-      <c r="D53"/>
-      <c r="E53"/>
-      <c r="F53"/>
-      <c r="G53"/>
-      <c r="H53"/>
-    </row>
-    <row r="54" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54"/>
-      <c r="B54"/>
-      <c r="C54"/>
-      <c r="D54"/>
-      <c r="E54"/>
-      <c r="F54"/>
-      <c r="G54"/>
-      <c r="H54"/>
-    </row>
-    <row r="55" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55"/>
-      <c r="B55"/>
-      <c r="C55"/>
-      <c r="D55"/>
-      <c r="E55"/>
-      <c r="F55"/>
-      <c r="G55"/>
-      <c r="H55"/>
-    </row>
-    <row r="56" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56"/>
-      <c r="B56"/>
-      <c r="C56"/>
-      <c r="D56"/>
-      <c r="E56"/>
-      <c r="F56"/>
-      <c r="G56"/>
-      <c r="H56"/>
-    </row>
-    <row r="57" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57"/>
-      <c r="B57"/>
-      <c r="C57"/>
-      <c r="D57"/>
-      <c r="E57"/>
-      <c r="F57"/>
-      <c r="G57"/>
-      <c r="H57"/>
-    </row>
-    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58"/>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
-      <c r="E58"/>
-      <c r="F58"/>
-      <c r="G58"/>
-      <c r="H58"/>
+      <c r="A42" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="13">
+        <v>4</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="D42" s="15">
+        <v>12</v>
+      </c>
+      <c r="E42" s="15">
+        <v>32</v>
+      </c>
+      <c r="F42" s="15">
+        <v>48</v>
+      </c>
+      <c r="G42" s="15">
+        <v>256</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="13">
+        <v>4</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="13">
+        <v>4</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="13">
+        <v>4</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46" s="13">
+        <v>4</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="G46" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="13">
+        <v>4</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F47" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="13">
+        <v>4</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F48" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="G48" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="13">
+        <v>4</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="G49" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="13">
+        <v>4</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="13">
+        <v>5</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="D51" s="16">
+        <v>255255255128</v>
+      </c>
+      <c r="E51" s="16">
+        <v>255255255192</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="G51" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="H51" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="13">
+        <v>5</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D52" s="16">
+        <v>255255255240</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="F52" s="16">
+        <v>255255255224</v>
+      </c>
+      <c r="G52" s="16">
+        <v>255255255192</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="13">
+        <v>5</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B54" s="13">
+        <v>5</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="D54" s="15">
+        <v>100</v>
+      </c>
+      <c r="E54" s="15">
+        <v>1000</v>
+      </c>
+      <c r="F54" s="15">
+        <v>200</v>
+      </c>
+      <c r="G54" s="15">
+        <v>2000</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="13">
+        <v>5</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="G55" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="H55" s="12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="13">
+        <v>5</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="G56" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="6" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="13">
+        <v>5</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="G57" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="H57" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="13">
+        <v>5</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="H58" s="12" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="59" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59"/>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
-      <c r="E59"/>
-      <c r="F59"/>
-      <c r="G59"/>
-      <c r="H59"/>
-    </row>
-    <row r="60" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60"/>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
-      <c r="E60"/>
-      <c r="F60"/>
-      <c r="G60"/>
-      <c r="H60"/>
-    </row>
-    <row r="61" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61"/>
-      <c r="B61"/>
-      <c r="C61"/>
-      <c r="D61"/>
-      <c r="E61"/>
-      <c r="F61"/>
-      <c r="G61"/>
-      <c r="H61"/>
-    </row>
-    <row r="62" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62"/>
-      <c r="B62"/>
-      <c r="C62"/>
-      <c r="D62"/>
-      <c r="E62"/>
-      <c r="F62"/>
-      <c r="G62"/>
-      <c r="H62"/>
-    </row>
-    <row r="63" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63"/>
-      <c r="B63"/>
-      <c r="C63"/>
-      <c r="D63"/>
-      <c r="E63"/>
-      <c r="F63"/>
-      <c r="G63"/>
-      <c r="H63"/>
-    </row>
-    <row r="64" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64"/>
-      <c r="B64"/>
-      <c r="C64"/>
-      <c r="D64"/>
-      <c r="E64"/>
-      <c r="F64"/>
-      <c r="G64"/>
-      <c r="H64"/>
-    </row>
-    <row r="65" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65"/>
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-      <c r="G65"/>
-      <c r="H65"/>
+      <c r="A59" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="13">
+        <v>6</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="G59" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B60" s="13">
+        <v>6</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F60" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="G60" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="H60" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B61" s="13">
+        <v>6</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="G61" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B62" s="13">
+        <v>6</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="G62" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="H62" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="13">
+        <v>6</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="G63" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B64" s="13">
+        <v>6</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="G64" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="H64" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B65" s="13">
+        <v>6</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="E65" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="66" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66"/>
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-      <c r="E66"/>
-      <c r="F66"/>
-      <c r="G66"/>
-      <c r="H66"/>
-    </row>
-    <row r="67" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67"/>
-      <c r="B67"/>
-      <c r="C67"/>
-      <c r="D67"/>
-      <c r="E67"/>
-      <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-    </row>
-    <row r="68" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68"/>
-      <c r="B68"/>
-      <c r="C68"/>
-      <c r="D68"/>
-      <c r="E68"/>
-      <c r="F68"/>
-      <c r="G68"/>
-      <c r="H68"/>
+      <c r="A66" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B66" s="13">
+        <v>7</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="E66" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G66" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="H66" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="13">
+        <v>7</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="E67" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="F67" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="13">
+        <v>7</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="F68" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="69" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69"/>
-      <c r="B69"/>
-      <c r="C69"/>
-      <c r="D69"/>
-      <c r="E69"/>
-      <c r="F69"/>
-      <c r="G69"/>
-      <c r="H69"/>
-    </row>
-    <row r="70" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70"/>
-      <c r="B70"/>
-      <c r="C70"/>
-      <c r="D70"/>
-      <c r="E70"/>
-      <c r="F70"/>
-      <c r="G70"/>
-      <c r="H70"/>
-    </row>
-    <row r="71" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71"/>
-      <c r="B71"/>
-      <c r="C71"/>
-      <c r="D71"/>
-      <c r="E71"/>
-      <c r="F71"/>
-      <c r="G71"/>
-      <c r="H71"/>
+      <c r="A69" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="13">
+        <v>7</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="G69" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70" s="13">
+        <v>7</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="G70" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="13">
+        <v>7</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="G71" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="72" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72"/>
@@ -2289,13 +3987,13 @@
           <x14:formula1>
             <xm:f>Questions_types!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A122:A1048576 A2:A14</xm:sqref>
+          <xm:sqref>A122:A1048576 A2:A71</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Questions_types!$B$2:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B1:B14 B122:B1048576</xm:sqref>
+          <xm:sqref>B122:B1048576 B1:B71</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>